<commit_message>
Finalización CRUD Prospectos - Auditoria Usuarios - Archivo excel Prospectos definido
* Falta agregar asignacion ProspectosUsuarios
* Terminar CambiarClave (falta halar id de usuario logeado)
* Falta Editar Prospecto (update segun el id del prospecto)
</commit_message>
<xml_diff>
--- a/prospectos.xlsx
+++ b/prospectos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOEM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\Documents\NetBeansProjects\SEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>correo</t>
   </si>
@@ -41,10 +41,40 @@
     <t>establecimientoProveniente</t>
   </si>
   <si>
-    <t>estado</t>
-  </si>
-  <si>
     <t>captador</t>
+  </si>
+  <si>
+    <t>cedula</t>
+  </si>
+  <si>
+    <t>celular</t>
+  </si>
+  <si>
+    <t>casa</t>
+  </si>
+  <si>
+    <t>pega</t>
+  </si>
+  <si>
+    <t>092</t>
+  </si>
+  <si>
+    <t>jda</t>
+  </si>
+  <si>
+    <t>jas</t>
+  </si>
+  <si>
+    <t>01923</t>
+  </si>
+  <si>
+    <t>0923</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>asf</t>
   </si>
 </sst>
 </file>
@@ -80,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,39 +393,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="5" max="6" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalización Asignacion individual, Campos auditoria a tabla prospectos, Excel validado (Ojo: los estilos podrían estar descuadrados)
Agregado:
* Botón descarga matriz prospectos
* Archivo excel modificado y con respectivas validaciones
* Asignaciones individuales
* Campos de auditorias para la tabla prospectos
* Asignación de Prospectos muestra DataGrid sólo de prospectos sin asignar.

Faltante:
* Falta agregar asignacion ProspectosUsuarios multiple
* Terminar CambiarClave (falta halar id de usuario logeado)
* Falta validar los registros repetidos al subir archivo excel
</commit_message>
<xml_diff>
--- a/prospectos.xlsx
+++ b/prospectos.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\Documents\NetBeansProjects\SEV\"/>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$4</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,8 +26,144 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>usuario1</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Número de cédula del prospecto, obligatorio.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Canal de captación, escribirlo correctamente.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Escribir uno o los dos nombres del prospecto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Escribir uno o los dos apellidos del prospecto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Número de celular del prospecto, campo opcional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Número de domicilio del prospecto, opcional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Correo electrónico del prospecto, opcional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>De donde proviene el prospecto, aplica tanto a colegios como empresas.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Número de cédula del que captó a dicho prospecto.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>correo</t>
   </si>
@@ -53,35 +192,62 @@
     <t>casa</t>
   </si>
   <si>
-    <t>pega</t>
-  </si>
-  <si>
-    <t>092</t>
-  </si>
-  <si>
-    <t>jda</t>
-  </si>
-  <si>
-    <t>jas</t>
-  </si>
-  <si>
-    <t>01923</t>
-  </si>
-  <si>
-    <t>0923</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>asf</t>
+    <t>FERIAS</t>
+  </si>
+  <si>
+    <t>0916478957</t>
+  </si>
+  <si>
+    <t>09976123487</t>
+  </si>
+  <si>
+    <t>042461928</t>
+  </si>
+  <si>
+    <t>csanchez@hotmail.com</t>
+  </si>
+  <si>
+    <t>0926520917</t>
+  </si>
+  <si>
+    <t>0939379562</t>
+  </si>
+  <si>
+    <t>042568796</t>
+  </si>
+  <si>
+    <t>alasdasd@gmail.com</t>
+  </si>
+  <si>
+    <t>0926520918</t>
+  </si>
+  <si>
+    <t>0926930504</t>
+  </si>
+  <si>
+    <t>CARLOS</t>
+  </si>
+  <si>
+    <t>SANCHEZ</t>
+  </si>
+  <si>
+    <t>AXEL</t>
+  </si>
+  <si>
+    <t>LATORRE</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>SEKKKKK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,16 +255,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,15 +307,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Entrada" xfId="2" builtinId="20"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,80 +621,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="5" max="6" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5"/>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar mayúsculas" error="Debes escribir este dato en mayúscula." sqref="B3:B1048576">
+      <formula1>EXACT(B3,UPPER(B3))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar en mayúsculas" error="Debes escribir este dato en mayúscula." sqref="B2">
+      <formula1>EXACT(B2,UPPER(B2))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar en mayúscula" error="Debes escribir este dato en mayúscula." sqref="C2:D1048576 H2:H1048576">
+      <formula1>EXACT(C2,UPPER(C2))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se añadieron los siguientes cambios:
* Cambiar contraseña: agregar text de volver a escribir contraseña
* Asignación Prospectos - Asignación masiva (verificar)
</commit_message>
<xml_diff>
--- a/prospectos.xlsx
+++ b/prospectos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>correo</t>
   </si>
@@ -241,6 +241,27 @@
   </si>
   <si>
     <t>SEKKKKK</t>
+  </si>
+  <si>
+    <t>0642575948</t>
+  </si>
+  <si>
+    <t>JUAN</t>
+  </si>
+  <si>
+    <t>COBOS</t>
+  </si>
+  <si>
+    <t>0994135784</t>
+  </si>
+  <si>
+    <t>115465477</t>
+  </si>
+  <si>
+    <t>jcobos@gmail.com</t>
+  </si>
+  <si>
+    <t>COPOL</t>
   </si>
 </sst>
 </file>
@@ -623,10 +644,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,46 +748,43 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>19</v>
+      <c r="A4" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5"/>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar en mayúsculas" error="Debes escribir este dato en mayúscula." sqref="B2">
+      <formula1>EXACT(B2,UPPER(B2))</formula1>
+    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar mayúsculas" error="Debes escribir este dato en mayúscula." sqref="B3:B1048576">
       <formula1>EXACT(B3,UPPER(B3))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar en mayúsculas" error="Debes escribir este dato en mayúscula." sqref="B2">
-      <formula1>EXACT(B2,UPPER(B2))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar en mayúscula" error="Debes escribir este dato en mayúscula." sqref="C2:D1048576 H2:H1048576">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Ingresar en mayúscula" error="Debes escribir este dato en mayúscula." sqref="H2:H1048576 C2:D1048576">
       <formula1>EXACT(C2,UPPER(C2))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>